<commit_message>
Revisioni files in base a ultimi feedback
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111SANTECXXXXX/santec_vendor/santec_ecaresuite/5.0.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111SANTECXXXXX/santec_vendor/santec_ecaresuite/5.0.0/report-checklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sorgenti\it-fse-accreditamento\GATEWAY\S1#111SANTECXXXXX\santec_vendor\santec_ecaresuite\5.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sorgenti\it-fse-accreditamento\GATEWAY\S1#111SANTECXXXXX\santec_vendor\santec_ecaresuite\5.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B95CBCC-4B2B-448A-A6F4-1792B49E0587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="150" windowWidth="35835" windowHeight="19005"/>
+    <workbookView xWindow="1380" yWindow="4410" windowWidth="43830" windowHeight="14280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="672">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -2688,15 +2689,6 @@
     <t>2023-04-29T20:34:40Z</t>
   </si>
   <si>
-    <t>6740f196bcfbe753</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.492147354ac88d5a51e9e9de8b19845884e7fb51d47d9a18e62898eac220e0c0.ac3720b80a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-30T00:08:02Z</t>
-  </si>
-  <si>
     <t>03f3677a849edff5</t>
   </si>
   <si>
@@ -3007,12 +2999,233 @@
   </si>
   <si>
     <t>Le sezioni di CDA2 presenti nel test case non vengono gestite da applicativo</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-10-02T14:07:14Z</t>
+  </si>
+  <si>
+    <t>59cba27a214c4915</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a6e975b8c0a216bbe459bb3e549c8a9208524814ec3b1c552f33939ae03f642b.93d93aee24^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
+  </si>
+  <si>
+    <t>2023-10-02T14:25:03Z</t>
+  </si>
+  <si>
+    <t>492869e52f88a3c7</t>
+  </si>
+  <si>
+    <t>Il gateway di validazione FSE2.0 non è accessibile. Contattare l'amministratore di sistema.</t>
+  </si>
+  <si>
+    <t>L'amministratore di sistema ha la possibilita di modificare la configurazione in base alle informazioni di dettaglio contenute nei log</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
+  </si>
+  <si>
+    <t>2023-10-02T14:29:42Z</t>
+  </si>
+  <si>
+    <t>9fcaf1057c62bd47</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_LDO_TIMEOUT</t>
+  </si>
+  <si>
+    <t>Il gateway di validazione FSE2.0 non è raggiungibile, riprovare più tardi</t>
+  </si>
+  <si>
+    <t>L'evento di timeout viene registrato nei log a disposizione dell'amministratore di sistema che può controllare eventuali problemi di connettività</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>2023-10-02T14:48:15Z</t>
+  </si>
+  <si>
+    <t>180c09316abfb18a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a6e975b8c0a216bbe459bb3e549c8a9208524814ec3b1c552f33939ae03f642b.75dc76ba8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>2023-10-02T14:57:03Z</t>
+  </si>
+  <si>
+    <t>1b88cf91122fb284</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a6e975b8c0a216bbe459bb3e549c8a9208524814ec3b1c552f33939ae03f642b.bd6b7f36da^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT7_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>2023-10-02T15:06:26Z</t>
+  </si>
+  <si>
+    <t>ed0ccc07fab6f8c1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.a6e975b8c0a216bbe459bb3e549c8a9208524814ec3b1c552f33939ae03f642b.93d1baadfa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il gateway di validazione FSE 2.0 ha riscontrato un livello di confidenzialità  del documento non corretto.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'errore viene prevenuto dalla logica interna dell'applicativo che non permette l'inserimento di anagrafiche dei pazienti senza il comune di residenza.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'errore viene prevenuto dalla logica interna dell'applicativo che non permette l'inserimento di anagrafiche dei pazienti non anonimi senza il nome.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'errore viene prevenuto dalla logica interna dell'applicativo che non permette l'inserimento di anagrafiche dei pazienti con sesso diverso da "maschio", "femmina" e "indifferenziato"</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT11_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'errore viene prevenuto dalla logica interna dell'applicativo che non permette l'inserimento di un lettera di dimissione senza la determinazione di almeno una diagnosi di dimissione.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'errore viene prevenuto dalla logica interna dell'applicativo che non permette l'inserimento di un lettera di dimissione senza un testo relativo al decorso ospedaliero.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT13_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'applicativo non gestisce i tag  CDA2 relativi al test.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT15_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>L'errore viene prevenuto dalla logica interna dell'applicativo che non permette l'inserimento di una diagnosi di ingresso non codificata icd9cm.</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -3381,12 +3594,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle name="Sheet1-style" pivot="0" count="3">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="firstRowStripe" dxfId="4"/>
       <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
-    <tableStyle name="Sheet1-style 2" pivot="0" count="3">
+    <tableStyle name="Sheet1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -3404,18 +3617,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:A3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:A3">
   <tableColumns count="1">
-    <tableColumn id="1" name="ESITO"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ESITO"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="B1:B3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B1:B3">
   <tableColumns count="1">
-    <tableColumn id="1" name="APPLICABILITA'"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="APPLICABILITA'"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3618,15 +3831,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T859"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C229" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B238" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K239" sqref="K239"/>
+      <selection pane="bottomRight" activeCell="L211" sqref="L211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9816,13 +10029,13 @@
         <v>45096</v>
       </c>
       <c r="G184" s="15" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="H184" s="15" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="I184" s="15" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J184" s="16" t="s">
         <v>396</v>
@@ -9835,13 +10048,13 @@
         <v>396</v>
       </c>
       <c r="N184" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="O184" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P184" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q184" s="16" t="s">
         <v>495</v>
@@ -9872,13 +10085,13 @@
         <v>45096</v>
       </c>
       <c r="G185" s="15" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="H185" s="15" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="I185" s="15" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J185" s="16" t="s">
         <v>396</v>
@@ -9891,13 +10104,13 @@
         <v>396</v>
       </c>
       <c r="N185" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="O185" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P185" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q185" s="16" t="s">
         <v>495</v>
@@ -9928,7 +10141,7 @@
         <v>45096</v>
       </c>
       <c r="G186" s="15" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H186" s="15"/>
       <c r="I186" s="15"/>
@@ -9943,13 +10156,13 @@
         <v>396</v>
       </c>
       <c r="N186" s="16" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="O186" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P186" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q186" s="16" t="s">
         <v>495</v>
@@ -9982,13 +10195,13 @@
         <v>45096</v>
       </c>
       <c r="G187" s="15" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="H187" s="15" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="I187" s="15" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="J187" s="16" t="s">
         <v>396</v>
@@ -10032,7 +10245,7 @@
         <v>497</v>
       </c>
       <c r="K188" s="16" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L188" s="16"/>
       <c r="M188" s="16"/>
@@ -10070,7 +10283,7 @@
         <v>497</v>
       </c>
       <c r="K189" s="16" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L189" s="16"/>
       <c r="M189" s="16"/>
@@ -10108,7 +10321,7 @@
         <v>497</v>
       </c>
       <c r="K190" s="16" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L190" s="16"/>
       <c r="M190" s="16"/>
@@ -10142,13 +10355,13 @@
         <v>45096</v>
       </c>
       <c r="G191" s="15" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="H191" s="15" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="I191" s="15" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J191" s="16" t="s">
         <v>396</v>
@@ -10161,13 +10374,13 @@
         <v>396</v>
       </c>
       <c r="N191" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O191" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P191" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q191" s="16" t="s">
         <v>495</v>
@@ -10198,13 +10411,13 @@
         <v>45096</v>
       </c>
       <c r="G192" s="15" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="H192" s="15" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="I192" s="15" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="J192" s="16" t="s">
         <v>396</v>
@@ -10217,13 +10430,13 @@
         <v>396</v>
       </c>
       <c r="N192" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O192" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P192" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q192" s="16" t="s">
         <v>495</v>
@@ -10254,13 +10467,13 @@
         <v>45096</v>
       </c>
       <c r="G193" s="15" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="H193" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="I193" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="J193" s="16" t="s">
         <v>396</v>
@@ -10273,13 +10486,13 @@
         <v>396</v>
       </c>
       <c r="N193" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O193" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P193" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q193" s="16" t="s">
         <v>495</v>
@@ -10310,13 +10523,13 @@
         <v>45096</v>
       </c>
       <c r="G194" s="15" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="H194" s="15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="I194" s="15" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="J194" s="16" t="s">
         <v>396</v>
@@ -10329,13 +10542,13 @@
         <v>396</v>
       </c>
       <c r="N194" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O194" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P194" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q194" s="16" t="s">
         <v>495</v>
@@ -10366,13 +10579,13 @@
         <v>45096</v>
       </c>
       <c r="G195" s="15" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H195" s="15" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="I195" s="15" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="J195" s="16" t="s">
         <v>396</v>
@@ -10385,13 +10598,13 @@
         <v>396</v>
       </c>
       <c r="N195" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O195" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P195" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q195" s="16" t="s">
         <v>495</v>
@@ -10422,13 +10635,13 @@
         <v>45096</v>
       </c>
       <c r="G196" s="15" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="H196" s="15" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I196" s="15" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J196" s="16" t="s">
         <v>396</v>
@@ -10441,13 +10654,13 @@
         <v>396</v>
       </c>
       <c r="N196" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O196" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P196" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q196" s="16" t="s">
         <v>495</v>
@@ -10482,7 +10695,7 @@
         <v>497</v>
       </c>
       <c r="K197" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L197" s="16"/>
       <c r="M197" s="16"/>
@@ -10520,7 +10733,7 @@
         <v>497</v>
       </c>
       <c r="K198" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L198" s="16"/>
       <c r="M198" s="16"/>
@@ -10558,7 +10771,7 @@
         <v>497</v>
       </c>
       <c r="K199" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L199" s="16"/>
       <c r="M199" s="16"/>
@@ -10592,13 +10805,13 @@
         <v>45096</v>
       </c>
       <c r="G200" s="15" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="H200" s="15" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="I200" s="15" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="J200" s="16" t="s">
         <v>396</v>
@@ -10611,13 +10824,13 @@
         <v>396</v>
       </c>
       <c r="N200" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O200" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P200" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q200" s="16" t="s">
         <v>495</v>
@@ -10648,13 +10861,13 @@
         <v>45096</v>
       </c>
       <c r="G201" s="15" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H201" s="15" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="I201" s="15" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="J201" s="16" t="s">
         <v>396</v>
@@ -10667,13 +10880,13 @@
         <v>396</v>
       </c>
       <c r="N201" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O201" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P201" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q201" s="16" t="s">
         <v>495</v>
@@ -10708,7 +10921,7 @@
         <v>497</v>
       </c>
       <c r="K202" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L202" s="16"/>
       <c r="M202" s="16"/>
@@ -10746,7 +10959,7 @@
         <v>497</v>
       </c>
       <c r="K203" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L203" s="16"/>
       <c r="M203" s="16"/>
@@ -10784,7 +10997,7 @@
         <v>497</v>
       </c>
       <c r="K204" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L204" s="16"/>
       <c r="M204" s="16"/>
@@ -10822,7 +11035,7 @@
         <v>497</v>
       </c>
       <c r="K205" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L205" s="16"/>
       <c r="M205" s="16"/>
@@ -10860,7 +11073,7 @@
         <v>497</v>
       </c>
       <c r="K206" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L206" s="16"/>
       <c r="M206" s="16"/>
@@ -10898,7 +11111,7 @@
         <v>497</v>
       </c>
       <c r="K207" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L207" s="16"/>
       <c r="M207" s="16"/>
@@ -10936,7 +11149,7 @@
         <v>497</v>
       </c>
       <c r="K208" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L208" s="16"/>
       <c r="M208" s="16"/>
@@ -10970,13 +11183,13 @@
         <v>45096</v>
       </c>
       <c r="G209" s="15" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="H209" s="15" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="I209" s="15" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J209" s="16" t="s">
         <v>396</v>
@@ -10989,13 +11202,13 @@
         <v>396</v>
       </c>
       <c r="N209" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O209" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P209" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q209" s="16" t="s">
         <v>495</v>
@@ -11068,30 +11281,22 @@
       <c r="E211" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="F211" s="14">
-        <v>45046</v>
-      </c>
-      <c r="G211" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="H211" s="15" t="s">
-        <v>505</v>
-      </c>
-      <c r="I211" s="15" t="s">
-        <v>506</v>
-      </c>
+      <c r="F211" s="14"/>
+      <c r="G211" s="15"/>
+      <c r="H211" s="15"/>
+      <c r="I211" s="15"/>
       <c r="J211" s="16" t="s">
-        <v>396</v>
-      </c>
-      <c r="K211" s="16"/>
+        <v>497</v>
+      </c>
+      <c r="K211" s="16" t="s">
+        <v>576</v>
+      </c>
       <c r="L211" s="16"/>
       <c r="M211" s="16"/>
       <c r="N211" s="16"/>
       <c r="O211" s="16"/>
       <c r="P211" s="16"/>
-      <c r="Q211" s="16" t="s">
-        <v>495</v>
-      </c>
+      <c r="Q211" s="16"/>
       <c r="R211" s="17"/>
       <c r="S211" s="18"/>
       <c r="T211" s="19" t="s">
@@ -11122,7 +11327,7 @@
         <v>497</v>
       </c>
       <c r="K212" s="16" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L212" s="16"/>
       <c r="M212" s="16"/>
@@ -11160,7 +11365,7 @@
         <v>497</v>
       </c>
       <c r="K213" s="16" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L213" s="16"/>
       <c r="M213" s="16"/>
@@ -11194,13 +11399,13 @@
         <v>45046</v>
       </c>
       <c r="G214" s="15" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="H214" s="15" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I214" s="15" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J214" s="16" t="s">
         <v>396</v>
@@ -11213,13 +11418,13 @@
         <v>396</v>
       </c>
       <c r="N214" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="O214" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P214" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q214" s="16" t="s">
         <v>495</v>
@@ -11250,13 +11455,13 @@
         <v>45046</v>
       </c>
       <c r="G215" s="15" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H215" s="15" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="I215" s="15" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J215" s="16" t="s">
         <v>396</v>
@@ -11269,13 +11474,13 @@
         <v>396</v>
       </c>
       <c r="N215" s="16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="O215" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P215" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q215" s="16" t="s">
         <v>495</v>
@@ -11306,7 +11511,7 @@
         <v>45046</v>
       </c>
       <c r="G216" s="15" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H216" s="15"/>
       <c r="I216" s="15"/>
@@ -11321,13 +11526,13 @@
         <v>396</v>
       </c>
       <c r="N216" s="16" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="O216" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P216" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q216" s="16" t="s">
         <v>495</v>
@@ -11360,13 +11565,13 @@
         <v>45046</v>
       </c>
       <c r="G217" s="15" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H217" s="15" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I217" s="15" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="J217" s="16" t="s">
         <v>396</v>
@@ -11379,13 +11584,13 @@
         <v>396</v>
       </c>
       <c r="N217" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O217" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P217" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q217" s="16" t="s">
         <v>495</v>
@@ -11416,13 +11621,13 @@
         <v>45046</v>
       </c>
       <c r="G218" s="15" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="H218" s="15" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I218" s="15" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="J218" s="16" t="s">
         <v>396</v>
@@ -11435,13 +11640,13 @@
         <v>396</v>
       </c>
       <c r="N218" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O218" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P218" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q218" s="16" t="s">
         <v>495</v>
@@ -11472,13 +11677,13 @@
         <v>45046</v>
       </c>
       <c r="G219" s="15" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H219" s="15" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I219" s="15" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="J219" s="16" t="s">
         <v>396</v>
@@ -11491,13 +11696,13 @@
         <v>396</v>
       </c>
       <c r="N219" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O219" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P219" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q219" s="16" t="s">
         <v>495</v>
@@ -11528,13 +11733,13 @@
         <v>45046</v>
       </c>
       <c r="G220" s="15" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H220" s="15" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="I220" s="15" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="J220" s="16" t="s">
         <v>396</v>
@@ -11547,13 +11752,13 @@
         <v>396</v>
       </c>
       <c r="N220" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O220" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P220" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q220" s="16" t="s">
         <v>495</v>
@@ -11584,13 +11789,13 @@
         <v>45046</v>
       </c>
       <c r="G221" s="15" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="H221" s="15" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="I221" s="15" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J221" s="16" t="s">
         <v>396</v>
@@ -11603,13 +11808,13 @@
         <v>396</v>
       </c>
       <c r="N221" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O221" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P221" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q221" s="16" t="s">
         <v>495</v>
@@ -11640,13 +11845,13 @@
         <v>45046</v>
       </c>
       <c r="G222" s="15" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H222" s="15" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I222" s="15" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="J222" s="16" t="s">
         <v>396</v>
@@ -11659,13 +11864,13 @@
         <v>396</v>
       </c>
       <c r="N222" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O222" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P222" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q222" s="16" t="s">
         <v>495</v>
@@ -11696,13 +11901,13 @@
         <v>45046</v>
       </c>
       <c r="G223" s="15" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H223" s="15" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I223" s="15" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J223" s="16" t="s">
         <v>396</v>
@@ -11715,13 +11920,13 @@
         <v>396</v>
       </c>
       <c r="N223" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O223" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P223" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q223" s="16" t="s">
         <v>495</v>
@@ -11752,13 +11957,13 @@
         <v>45046</v>
       </c>
       <c r="G224" s="15" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H224" s="15" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="I224" s="15" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J224" s="16" t="s">
         <v>396</v>
@@ -11771,13 +11976,13 @@
         <v>396</v>
       </c>
       <c r="N224" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O224" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P224" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q224" s="16" t="s">
         <v>495</v>
@@ -11808,13 +12013,13 @@
         <v>45048</v>
       </c>
       <c r="G225" s="15" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="H225" s="15" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="I225" s="15" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="J225" s="16" t="s">
         <v>396</v>
@@ -11827,13 +12032,13 @@
         <v>396</v>
       </c>
       <c r="N225" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O225" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P225" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q225" s="16" t="s">
         <v>495</v>
@@ -11864,13 +12069,13 @@
         <v>45048</v>
       </c>
       <c r="G226" s="15" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="H226" s="15" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="I226" s="15" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J226" s="16" t="s">
         <v>396</v>
@@ -11883,13 +12088,13 @@
         <v>396</v>
       </c>
       <c r="N226" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O226" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P226" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q226" s="16" t="s">
         <v>495</v>
@@ -11920,13 +12125,13 @@
         <v>45048</v>
       </c>
       <c r="G227" s="15" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="H227" s="15" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="I227" s="15" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J227" s="16" t="s">
         <v>396</v>
@@ -11939,13 +12144,13 @@
         <v>396</v>
       </c>
       <c r="N227" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O227" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P227" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q227" s="16" t="s">
         <v>495</v>
@@ -11976,13 +12181,13 @@
         <v>45048</v>
       </c>
       <c r="G228" s="15" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H228" s="15" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="I228" s="15" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="J228" s="16" t="s">
         <v>396</v>
@@ -11995,13 +12200,13 @@
         <v>396</v>
       </c>
       <c r="N228" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O228" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P228" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q228" s="16" t="s">
         <v>495</v>
@@ -12032,13 +12237,13 @@
         <v>45048</v>
       </c>
       <c r="G229" s="15" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="H229" s="15" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="I229" s="15" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="J229" s="16" t="s">
         <v>396</v>
@@ -12051,13 +12256,13 @@
         <v>396</v>
       </c>
       <c r="N229" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O229" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P229" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q229" s="16" t="s">
         <v>495</v>
@@ -12092,7 +12297,7 @@
         <v>497</v>
       </c>
       <c r="K230" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L230" s="16"/>
       <c r="M230" s="16"/>
@@ -12130,7 +12335,7 @@
         <v>497</v>
       </c>
       <c r="K231" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L231" s="16"/>
       <c r="M231" s="16"/>
@@ -12164,13 +12369,13 @@
         <v>45048</v>
       </c>
       <c r="G232" s="15" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H232" s="15" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="I232" s="15" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="J232" s="16" t="s">
         <v>396</v>
@@ -12183,13 +12388,13 @@
         <v>396</v>
       </c>
       <c r="N232" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O232" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P232" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q232" s="16" t="s">
         <v>495</v>
@@ -12224,7 +12429,7 @@
         <v>497</v>
       </c>
       <c r="K233" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L233" s="16"/>
       <c r="M233" s="16"/>
@@ -12258,13 +12463,13 @@
         <v>45048</v>
       </c>
       <c r="G234" s="15" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="H234" s="15" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="I234" s="15" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="J234" s="16" t="s">
         <v>396</v>
@@ -12277,13 +12482,13 @@
         <v>396</v>
       </c>
       <c r="N234" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O234" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P234" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q234" s="16" t="s">
         <v>495</v>
@@ -12314,13 +12519,13 @@
         <v>45048</v>
       </c>
       <c r="G235" s="15" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="H235" s="15" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="I235" s="15" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="J235" s="16" t="s">
         <v>396</v>
@@ -12333,13 +12538,13 @@
         <v>396</v>
       </c>
       <c r="N235" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O235" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P235" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q235" s="16" t="s">
         <v>495</v>
@@ -12374,7 +12579,7 @@
         <v>497</v>
       </c>
       <c r="K236" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L236" s="16"/>
       <c r="M236" s="16"/>
@@ -12408,13 +12613,13 @@
         <v>45048</v>
       </c>
       <c r="G237" s="15" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="H237" s="15" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="I237" s="15" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="J237" s="16" t="s">
         <v>396</v>
@@ -12427,13 +12632,13 @@
         <v>396</v>
       </c>
       <c r="N237" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O237" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P237" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q237" s="16" t="s">
         <v>495</v>
@@ -12464,13 +12669,13 @@
         <v>45048</v>
       </c>
       <c r="G238" s="15" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H238" s="15" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="I238" s="15" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="J238" s="16" t="s">
         <v>396</v>
@@ -12483,13 +12688,13 @@
         <v>396</v>
       </c>
       <c r="N238" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O238" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P238" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q238" s="16" t="s">
         <v>495</v>
@@ -12520,13 +12725,13 @@
         <v>45048</v>
       </c>
       <c r="G239" s="15" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H239" s="15" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="I239" s="15" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="J239" s="16" t="s">
         <v>396</v>
@@ -12539,13 +12744,13 @@
         <v>396</v>
       </c>
       <c r="N239" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="O239" s="16" t="s">
         <v>396</v>
       </c>
       <c r="P239" s="16" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="Q239" s="16" t="s">
         <v>495</v>
@@ -12580,7 +12785,7 @@
         <v>497</v>
       </c>
       <c r="K240" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L240" s="16"/>
       <c r="M240" s="16"/>
@@ -12594,7 +12799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="120">
+    <row r="241" spans="1:20" ht="120.75" thickBot="1">
       <c r="A241" s="11">
         <v>146</v>
       </c>
@@ -12618,7 +12823,7 @@
         <v>497</v>
       </c>
       <c r="K241" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="L241" s="16"/>
       <c r="M241" s="16"/>
@@ -12632,330 +12837,843 @@
         <v>29</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F242" s="3"/>
-      <c r="G242" s="3"/>
-      <c r="H242" s="3"/>
-      <c r="I242" s="3"/>
-      <c r="J242" s="4"/>
-      <c r="K242" s="4"/>
-      <c r="L242" s="4"/>
-      <c r="M242" s="4"/>
-      <c r="N242" s="4"/>
-      <c r="O242" s="4"/>
-      <c r="P242" s="4"/>
-      <c r="Q242" s="4"/>
-      <c r="R242" s="5"/>
-      <c r="S242" s="1"/>
-      <c r="T242" s="6"/>
-    </row>
-    <row r="243" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F243" s="3"/>
-      <c r="G243" s="3"/>
-      <c r="H243" s="3"/>
-      <c r="I243" s="3"/>
-      <c r="J243" s="4"/>
-      <c r="K243" s="4"/>
-      <c r="L243" s="4"/>
-      <c r="M243" s="4"/>
-      <c r="N243" s="4"/>
-      <c r="O243" s="4"/>
-      <c r="P243" s="4"/>
-      <c r="Q243" s="4"/>
-      <c r="R243" s="5"/>
-      <c r="S243" s="1"/>
-      <c r="T243" s="6"/>
-    </row>
-    <row r="244" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F244" s="3"/>
-      <c r="G244" s="3"/>
-      <c r="H244" s="3"/>
-      <c r="I244" s="3"/>
-      <c r="J244" s="4"/>
-      <c r="K244" s="4"/>
-      <c r="L244" s="4"/>
-      <c r="M244" s="4"/>
-      <c r="N244" s="4"/>
-      <c r="O244" s="4"/>
-      <c r="P244" s="4"/>
-      <c r="Q244" s="4"/>
-      <c r="R244" s="5"/>
-      <c r="S244" s="1"/>
-      <c r="T244" s="6"/>
-    </row>
-    <row r="245" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F245" s="3"/>
-      <c r="G245" s="3"/>
-      <c r="H245" s="3"/>
-      <c r="I245" s="3"/>
-      <c r="J245" s="4"/>
-      <c r="K245" s="4"/>
-      <c r="L245" s="4"/>
-      <c r="M245" s="4"/>
-      <c r="N245" s="4"/>
-      <c r="O245" s="4"/>
-      <c r="P245" s="4"/>
-      <c r="Q245" s="4"/>
-      <c r="R245" s="5"/>
-      <c r="S245" s="1"/>
-      <c r="T245" s="6"/>
-    </row>
-    <row r="246" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F246" s="3"/>
-      <c r="G246" s="3"/>
-      <c r="H246" s="3"/>
-      <c r="I246" s="3"/>
-      <c r="J246" s="4"/>
-      <c r="K246" s="4"/>
-      <c r="L246" s="4"/>
-      <c r="M246" s="4"/>
-      <c r="N246" s="4"/>
-      <c r="O246" s="4"/>
-      <c r="P246" s="4"/>
-      <c r="Q246" s="4"/>
-      <c r="R246" s="5"/>
-      <c r="S246" s="1"/>
-      <c r="T246" s="6"/>
-    </row>
-    <row r="247" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F247" s="3"/>
-      <c r="G247" s="3"/>
-      <c r="H247" s="3"/>
-      <c r="I247" s="3"/>
-      <c r="J247" s="4"/>
-      <c r="K247" s="4"/>
-      <c r="L247" s="4"/>
-      <c r="M247" s="4"/>
-      <c r="N247" s="4"/>
-      <c r="O247" s="4"/>
-      <c r="P247" s="4"/>
-      <c r="Q247" s="4"/>
-      <c r="R247" s="5"/>
-      <c r="S247" s="1"/>
-      <c r="T247" s="6"/>
-    </row>
-    <row r="248" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F248" s="3"/>
-      <c r="G248" s="3"/>
-      <c r="H248" s="3"/>
-      <c r="I248" s="3"/>
-      <c r="J248" s="4"/>
-      <c r="K248" s="4"/>
-      <c r="L248" s="4"/>
-      <c r="M248" s="4"/>
-      <c r="N248" s="4"/>
-      <c r="O248" s="4"/>
-      <c r="P248" s="4"/>
-      <c r="Q248" s="4"/>
-      <c r="R248" s="5"/>
-      <c r="S248" s="1"/>
-      <c r="T248" s="6"/>
-    </row>
-    <row r="249" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F249" s="3"/>
-      <c r="G249" s="3"/>
-      <c r="H249" s="3"/>
-      <c r="I249" s="3"/>
-      <c r="J249" s="4"/>
-      <c r="K249" s="4"/>
-      <c r="L249" s="4"/>
-      <c r="M249" s="4"/>
-      <c r="N249" s="4"/>
-      <c r="O249" s="4"/>
-      <c r="P249" s="4"/>
-      <c r="Q249" s="4"/>
-      <c r="R249" s="5"/>
-      <c r="S249" s="1"/>
-      <c r="T249" s="6"/>
-    </row>
-    <row r="250" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F250" s="3"/>
-      <c r="G250" s="3"/>
-      <c r="H250" s="3"/>
-      <c r="I250" s="3"/>
-      <c r="J250" s="4"/>
-      <c r="K250" s="4"/>
-      <c r="L250" s="4"/>
-      <c r="M250" s="4"/>
-      <c r="N250" s="4"/>
-      <c r="O250" s="4"/>
-      <c r="P250" s="4"/>
-      <c r="Q250" s="4"/>
-      <c r="R250" s="5"/>
-      <c r="S250" s="1"/>
-      <c r="T250" s="6"/>
-    </row>
-    <row r="251" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F251" s="3"/>
-      <c r="G251" s="3"/>
-      <c r="H251" s="3"/>
-      <c r="I251" s="3"/>
-      <c r="J251" s="4"/>
-      <c r="K251" s="4"/>
-      <c r="L251" s="4"/>
-      <c r="M251" s="4"/>
-      <c r="N251" s="4"/>
-      <c r="O251" s="4"/>
-      <c r="P251" s="4"/>
-      <c r="Q251" s="4"/>
-      <c r="R251" s="5"/>
-      <c r="S251" s="1"/>
-      <c r="T251" s="6"/>
-    </row>
-    <row r="252" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F252" s="3"/>
-      <c r="G252" s="3"/>
-      <c r="H252" s="3"/>
-      <c r="I252" s="3"/>
-      <c r="J252" s="4"/>
-      <c r="K252" s="4"/>
-      <c r="L252" s="4"/>
-      <c r="M252" s="4"/>
-      <c r="N252" s="4"/>
-      <c r="O252" s="4"/>
-      <c r="P252" s="4"/>
-      <c r="Q252" s="4"/>
-      <c r="R252" s="5"/>
-      <c r="S252" s="1"/>
-      <c r="T252" s="6"/>
-    </row>
-    <row r="253" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F253" s="3"/>
-      <c r="G253" s="3"/>
-      <c r="H253" s="3"/>
-      <c r="I253" s="3"/>
-      <c r="J253" s="4"/>
-      <c r="K253" s="4"/>
-      <c r="L253" s="4"/>
-      <c r="M253" s="4"/>
-      <c r="N253" s="4"/>
-      <c r="O253" s="4"/>
-      <c r="P253" s="4"/>
-      <c r="Q253" s="4"/>
-      <c r="R253" s="5"/>
-      <c r="S253" s="1"/>
-      <c r="T253" s="6"/>
-    </row>
-    <row r="254" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F254" s="3"/>
-      <c r="G254" s="3"/>
-      <c r="H254" s="3"/>
-      <c r="I254" s="3"/>
-      <c r="J254" s="4"/>
-      <c r="K254" s="4"/>
-      <c r="L254" s="4"/>
-      <c r="M254" s="4"/>
-      <c r="N254" s="4"/>
-      <c r="O254" s="4"/>
-      <c r="P254" s="4"/>
-      <c r="Q254" s="4"/>
-      <c r="R254" s="5"/>
-      <c r="S254" s="1"/>
-      <c r="T254" s="6"/>
-    </row>
-    <row r="255" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F255" s="3"/>
-      <c r="G255" s="3"/>
-      <c r="H255" s="3"/>
-      <c r="I255" s="3"/>
-      <c r="J255" s="4"/>
-      <c r="K255" s="4"/>
-      <c r="L255" s="4"/>
-      <c r="M255" s="4"/>
-      <c r="N255" s="4"/>
-      <c r="O255" s="4"/>
-      <c r="P255" s="4"/>
-      <c r="Q255" s="4"/>
-      <c r="R255" s="5"/>
-      <c r="S255" s="1"/>
-      <c r="T255" s="6"/>
-    </row>
-    <row r="256" spans="1:20" ht="14.25" customHeight="1">
-      <c r="F256" s="3"/>
-      <c r="G256" s="3"/>
-      <c r="H256" s="3"/>
-      <c r="I256" s="3"/>
-      <c r="J256" s="4"/>
-      <c r="K256" s="4"/>
-      <c r="L256" s="4"/>
-      <c r="M256" s="4"/>
-      <c r="N256" s="4"/>
-      <c r="O256" s="4"/>
-      <c r="P256" s="4"/>
-      <c r="Q256" s="4"/>
-      <c r="R256" s="5"/>
-      <c r="S256" s="1"/>
-      <c r="T256" s="6"/>
-    </row>
-    <row r="257" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F257" s="3"/>
-      <c r="G257" s="3"/>
-      <c r="H257" s="3"/>
-      <c r="I257" s="3"/>
-      <c r="J257" s="4"/>
-      <c r="K257" s="4"/>
-      <c r="L257" s="4"/>
-      <c r="M257" s="4"/>
-      <c r="N257" s="4"/>
-      <c r="O257" s="4"/>
-      <c r="P257" s="4"/>
-      <c r="Q257" s="4"/>
-      <c r="R257" s="5"/>
-      <c r="S257" s="1"/>
-      <c r="T257" s="6"/>
-    </row>
-    <row r="258" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F258" s="3"/>
-      <c r="G258" s="3"/>
-      <c r="H258" s="3"/>
-      <c r="I258" s="3"/>
-      <c r="J258" s="4"/>
-      <c r="K258" s="4"/>
-      <c r="L258" s="4"/>
-      <c r="M258" s="4"/>
-      <c r="N258" s="4"/>
-      <c r="O258" s="4"/>
-      <c r="P258" s="4"/>
-      <c r="Q258" s="4"/>
-      <c r="R258" s="5"/>
-      <c r="S258" s="1"/>
-      <c r="T258" s="6"/>
-    </row>
-    <row r="259" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F259" s="3"/>
-      <c r="G259" s="3"/>
-      <c r="H259" s="3"/>
-      <c r="I259" s="3"/>
-      <c r="J259" s="4"/>
-      <c r="K259" s="4"/>
-      <c r="L259" s="4"/>
-      <c r="M259" s="4"/>
-      <c r="N259" s="4"/>
-      <c r="O259" s="4"/>
-      <c r="P259" s="4"/>
-      <c r="Q259" s="4"/>
-      <c r="R259" s="5"/>
-      <c r="S259" s="1"/>
-      <c r="T259" s="6"/>
-    </row>
-    <row r="260" spans="6:20" ht="14.25" customHeight="1">
-      <c r="F260" s="3"/>
-      <c r="G260" s="3"/>
-      <c r="H260" s="3"/>
-      <c r="I260" s="3"/>
-      <c r="J260" s="4"/>
-      <c r="K260" s="4"/>
-      <c r="L260" s="4"/>
-      <c r="M260" s="4"/>
-      <c r="N260" s="4"/>
-      <c r="O260" s="4"/>
-      <c r="P260" s="4"/>
-      <c r="Q260" s="4"/>
-      <c r="R260" s="5"/>
-      <c r="S260" s="1"/>
-      <c r="T260" s="6"/>
-    </row>
-    <row r="261" spans="6:20" ht="14.25" customHeight="1">
+    <row r="242" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A242" s="11">
+        <v>6</v>
+      </c>
+      <c r="B242" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C242" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D242" s="12" t="s">
+        <v>609</v>
+      </c>
+      <c r="E242" s="13" t="s">
+        <v>610</v>
+      </c>
+      <c r="F242" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G242" s="15" t="s">
+        <v>611</v>
+      </c>
+      <c r="H242" s="15" t="s">
+        <v>612</v>
+      </c>
+      <c r="I242" s="15" t="s">
+        <v>613</v>
+      </c>
+      <c r="J242" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K242" s="16"/>
+      <c r="L242" s="16"/>
+      <c r="M242" s="16"/>
+      <c r="N242" s="16"/>
+      <c r="O242" s="16"/>
+      <c r="P242" s="16"/>
+      <c r="Q242" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R242" s="17"/>
+      <c r="S242" s="18"/>
+      <c r="T242" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="243" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A243" s="11">
+        <v>7</v>
+      </c>
+      <c r="B243" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C243" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D243" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="E243" s="13" t="s">
+        <v>615</v>
+      </c>
+      <c r="F243" s="14"/>
+      <c r="G243" s="15"/>
+      <c r="H243" s="15"/>
+      <c r="I243" s="15"/>
+      <c r="J243" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K243" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="L243" s="16"/>
+      <c r="M243" s="16"/>
+      <c r="N243" s="16"/>
+      <c r="O243" s="16"/>
+      <c r="P243" s="16"/>
+      <c r="Q243" s="16"/>
+      <c r="R243" s="17"/>
+      <c r="S243" s="18"/>
+      <c r="T243" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="244" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A244" s="11">
+        <v>8</v>
+      </c>
+      <c r="B244" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C244" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D244" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="E244" s="13" t="s">
+        <v>617</v>
+      </c>
+      <c r="F244" s="14"/>
+      <c r="G244" s="15"/>
+      <c r="H244" s="15"/>
+      <c r="I244" s="15"/>
+      <c r="J244" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K244" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="L244" s="16"/>
+      <c r="M244" s="16"/>
+      <c r="N244" s="16"/>
+      <c r="O244" s="16"/>
+      <c r="P244" s="16"/>
+      <c r="Q244" s="16"/>
+      <c r="R244" s="17"/>
+      <c r="S244" s="18"/>
+      <c r="T244" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="245" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A245" s="11">
+        <v>9</v>
+      </c>
+      <c r="B245" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C245" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D245" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="E245" s="13" t="s">
+        <v>619</v>
+      </c>
+      <c r="F245" s="14"/>
+      <c r="G245" s="15"/>
+      <c r="H245" s="15"/>
+      <c r="I245" s="15"/>
+      <c r="J245" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K245" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="L245" s="16"/>
+      <c r="M245" s="16"/>
+      <c r="N245" s="16"/>
+      <c r="O245" s="16"/>
+      <c r="P245" s="16"/>
+      <c r="Q245" s="16"/>
+      <c r="R245" s="17"/>
+      <c r="S245" s="18"/>
+      <c r="T245" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="246" spans="1:20" ht="150.75" thickBot="1">
+      <c r="A246" s="11">
+        <v>29</v>
+      </c>
+      <c r="B246" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C246" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D246" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="E246" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="F246" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G246" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="H246" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="I246" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="J246" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K246" s="16"/>
+      <c r="L246" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="M246" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="N246" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="O246" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="P246" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q246" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R246" s="17"/>
+      <c r="S246" s="18"/>
+      <c r="T246" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="247" spans="1:20" ht="165.75" thickBot="1">
+      <c r="A247" s="11">
+        <v>37</v>
+      </c>
+      <c r="B247" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C247" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D247" s="12" t="s">
+        <v>625</v>
+      </c>
+      <c r="E247" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="F247" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G247" s="15" t="s">
+        <v>626</v>
+      </c>
+      <c r="H247" s="15" t="s">
+        <v>627</v>
+      </c>
+      <c r="I247" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="J247" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K247" s="16"/>
+      <c r="L247" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="M247" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="N247" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="O247" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="P247" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="Q247" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R247" s="17"/>
+      <c r="S247" s="18"/>
+      <c r="T247" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="248" spans="1:20" ht="105.75" thickBot="1">
+      <c r="A248" s="11">
+        <v>45</v>
+      </c>
+      <c r="B248" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C248" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D248" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="E248" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="F248" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G248" s="15" t="s">
+        <v>626</v>
+      </c>
+      <c r="H248" s="15"/>
+      <c r="I248" s="15"/>
+      <c r="J248" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K248" s="16"/>
+      <c r="L248" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="M248" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="N248" s="16" t="s">
+        <v>629</v>
+      </c>
+      <c r="O248" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="P248" s="16" t="s">
+        <v>630</v>
+      </c>
+      <c r="Q248" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R248" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="S248" s="18"/>
+      <c r="T248" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="249" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A249" s="11">
+        <v>63</v>
+      </c>
+      <c r="B249" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C249" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D249" s="12" t="s">
+        <v>631</v>
+      </c>
+      <c r="E249" s="13" t="s">
+        <v>632</v>
+      </c>
+      <c r="F249" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G249" s="15" t="s">
+        <v>633</v>
+      </c>
+      <c r="H249" s="15" t="s">
+        <v>634</v>
+      </c>
+      <c r="I249" s="15" t="s">
+        <v>635</v>
+      </c>
+      <c r="J249" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K249" s="16"/>
+      <c r="L249" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="M249" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="N249" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="O249" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="P249" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q249" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R249" s="17"/>
+      <c r="S249" s="18"/>
+      <c r="T249" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="250" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A250" s="11">
+        <v>64</v>
+      </c>
+      <c r="B250" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C250" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D250" s="12" t="s">
+        <v>636</v>
+      </c>
+      <c r="E250" s="13" t="s">
+        <v>637</v>
+      </c>
+      <c r="F250" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G250" s="15" t="s">
+        <v>638</v>
+      </c>
+      <c r="H250" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="I250" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="J250" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K250" s="16"/>
+      <c r="L250" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="M250" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="N250" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="O250" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="P250" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q250" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R250" s="17"/>
+      <c r="S250" s="18"/>
+      <c r="T250" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="251" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A251" s="11">
+        <v>65</v>
+      </c>
+      <c r="B251" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C251" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D251" s="12" t="s">
+        <v>641</v>
+      </c>
+      <c r="E251" s="13" t="s">
+        <v>642</v>
+      </c>
+      <c r="F251" s="14">
+        <v>45201</v>
+      </c>
+      <c r="G251" s="15" t="s">
+        <v>643</v>
+      </c>
+      <c r="H251" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="I251" s="15" t="s">
+        <v>645</v>
+      </c>
+      <c r="J251" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="K251" s="16"/>
+      <c r="L251" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="M251" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="N251" s="16" t="s">
+        <v>646</v>
+      </c>
+      <c r="O251" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="P251" s="16" t="s">
+        <v>509</v>
+      </c>
+      <c r="Q251" s="16" t="s">
+        <v>495</v>
+      </c>
+      <c r="R251" s="17"/>
+      <c r="S251" s="18"/>
+      <c r="T251" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="252" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A252" s="11">
+        <v>66</v>
+      </c>
+      <c r="B252" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C252" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D252" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="E252" s="13" t="s">
+        <v>648</v>
+      </c>
+      <c r="F252" s="14"/>
+      <c r="G252" s="15"/>
+      <c r="H252" s="15"/>
+      <c r="I252" s="15"/>
+      <c r="J252" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K252" s="16" t="s">
+        <v>649</v>
+      </c>
+      <c r="L252" s="16"/>
+      <c r="M252" s="16"/>
+      <c r="N252" s="16"/>
+      <c r="O252" s="16"/>
+      <c r="P252" s="16"/>
+      <c r="Q252" s="16"/>
+      <c r="R252" s="17"/>
+      <c r="S252" s="18"/>
+      <c r="T252" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="253" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A253" s="11">
+        <v>67</v>
+      </c>
+      <c r="B253" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C253" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D253" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="E253" s="13" t="s">
+        <v>651</v>
+      </c>
+      <c r="F253" s="14"/>
+      <c r="G253" s="15"/>
+      <c r="H253" s="15"/>
+      <c r="I253" s="15"/>
+      <c r="J253" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K253" s="16" t="s">
+        <v>652</v>
+      </c>
+      <c r="L253" s="16"/>
+      <c r="M253" s="16"/>
+      <c r="N253" s="16"/>
+      <c r="O253" s="16"/>
+      <c r="P253" s="16"/>
+      <c r="Q253" s="16"/>
+      <c r="R253" s="17"/>
+      <c r="S253" s="18"/>
+      <c r="T253" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="254" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A254" s="11">
+        <v>68</v>
+      </c>
+      <c r="B254" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C254" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D254" s="12" t="s">
+        <v>653</v>
+      </c>
+      <c r="E254" s="13" t="s">
+        <v>654</v>
+      </c>
+      <c r="F254" s="14"/>
+      <c r="G254" s="15"/>
+      <c r="H254" s="15"/>
+      <c r="I254" s="15"/>
+      <c r="J254" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K254" s="16" t="s">
+        <v>655</v>
+      </c>
+      <c r="L254" s="16"/>
+      <c r="M254" s="16"/>
+      <c r="N254" s="16"/>
+      <c r="O254" s="16"/>
+      <c r="P254" s="16"/>
+      <c r="Q254" s="16"/>
+      <c r="R254" s="17"/>
+      <c r="S254" s="18"/>
+      <c r="T254" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="255" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A255" s="11">
+        <v>69</v>
+      </c>
+      <c r="B255" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C255" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D255" s="12" t="s">
+        <v>656</v>
+      </c>
+      <c r="E255" s="13" t="s">
+        <v>657</v>
+      </c>
+      <c r="F255" s="14"/>
+      <c r="G255" s="15"/>
+      <c r="H255" s="15"/>
+      <c r="I255" s="15"/>
+      <c r="J255" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K255" s="16" t="s">
+        <v>658</v>
+      </c>
+      <c r="L255" s="16"/>
+      <c r="M255" s="16"/>
+      <c r="N255" s="16"/>
+      <c r="O255" s="16"/>
+      <c r="P255" s="16"/>
+      <c r="Q255" s="16"/>
+      <c r="R255" s="17"/>
+      <c r="S255" s="18"/>
+      <c r="T255" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="256" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A256" s="11">
+        <v>70</v>
+      </c>
+      <c r="B256" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C256" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D256" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="E256" s="13" t="s">
+        <v>660</v>
+      </c>
+      <c r="F256" s="14"/>
+      <c r="G256" s="15"/>
+      <c r="H256" s="15"/>
+      <c r="I256" s="15"/>
+      <c r="J256" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K256" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="L256" s="16"/>
+      <c r="M256" s="16"/>
+      <c r="N256" s="16"/>
+      <c r="O256" s="16"/>
+      <c r="P256" s="16"/>
+      <c r="Q256" s="16"/>
+      <c r="R256" s="17"/>
+      <c r="S256" s="18"/>
+      <c r="T256" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="257" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A257" s="11">
+        <v>71</v>
+      </c>
+      <c r="B257" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C257" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D257" s="12" t="s">
+        <v>662</v>
+      </c>
+      <c r="E257" s="13" t="s">
+        <v>663</v>
+      </c>
+      <c r="F257" s="14"/>
+      <c r="G257" s="15"/>
+      <c r="H257" s="15"/>
+      <c r="I257" s="15"/>
+      <c r="J257" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K257" s="16" t="s">
+        <v>664</v>
+      </c>
+      <c r="L257" s="16"/>
+      <c r="M257" s="16"/>
+      <c r="N257" s="16"/>
+      <c r="O257" s="16"/>
+      <c r="P257" s="16"/>
+      <c r="Q257" s="16"/>
+      <c r="R257" s="17"/>
+      <c r="S257" s="18"/>
+      <c r="T257" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="258" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A258" s="11">
+        <v>72</v>
+      </c>
+      <c r="B258" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C258" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D258" s="12" t="s">
+        <v>665</v>
+      </c>
+      <c r="E258" s="13" t="s">
+        <v>666</v>
+      </c>
+      <c r="F258" s="14"/>
+      <c r="G258" s="15"/>
+      <c r="H258" s="15"/>
+      <c r="I258" s="15"/>
+      <c r="J258" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K258" s="16" t="s">
+        <v>664</v>
+      </c>
+      <c r="L258" s="16"/>
+      <c r="M258" s="16"/>
+      <c r="N258" s="16"/>
+      <c r="O258" s="16"/>
+      <c r="P258" s="16"/>
+      <c r="Q258" s="16"/>
+      <c r="R258" s="17"/>
+      <c r="S258" s="18"/>
+      <c r="T258" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="259" spans="1:20" ht="120.75" thickBot="1">
+      <c r="A259" s="11">
+        <v>73</v>
+      </c>
+      <c r="B259" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C259" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D259" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="E259" s="13" t="s">
+        <v>668</v>
+      </c>
+      <c r="F259" s="14"/>
+      <c r="G259" s="15"/>
+      <c r="H259" s="15"/>
+      <c r="I259" s="15"/>
+      <c r="J259" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K259" s="16" t="s">
+        <v>669</v>
+      </c>
+      <c r="L259" s="16"/>
+      <c r="M259" s="16"/>
+      <c r="N259" s="16"/>
+      <c r="O259" s="16"/>
+      <c r="P259" s="16"/>
+      <c r="Q259" s="16"/>
+      <c r="R259" s="17"/>
+      <c r="S259" s="18"/>
+      <c r="T259" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="260" spans="1:20" ht="120">
+      <c r="A260" s="11">
+        <v>74</v>
+      </c>
+      <c r="B260" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C260" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D260" s="12" t="s">
+        <v>670</v>
+      </c>
+      <c r="E260" s="13" t="s">
+        <v>671</v>
+      </c>
+      <c r="F260" s="14"/>
+      <c r="G260" s="15"/>
+      <c r="H260" s="15"/>
+      <c r="I260" s="15"/>
+      <c r="J260" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="K260" s="16" t="s">
+        <v>664</v>
+      </c>
+      <c r="L260" s="16"/>
+      <c r="M260" s="16"/>
+      <c r="N260" s="16"/>
+      <c r="O260" s="16"/>
+      <c r="P260" s="16"/>
+      <c r="Q260" s="16"/>
+      <c r="R260" s="17"/>
+      <c r="S260" s="18"/>
+      <c r="T260" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="261" spans="1:20" ht="14.25" customHeight="1">
       <c r="F261" s="3"/>
       <c r="G261" s="3"/>
       <c r="H261" s="3"/>
@@ -12972,7 +13690,7 @@
       <c r="S261" s="1"/>
       <c r="T261" s="6"/>
     </row>
-    <row r="262" spans="6:20" ht="14.25" customHeight="1">
+    <row r="262" spans="1:20" ht="14.25" customHeight="1">
       <c r="F262" s="3"/>
       <c r="G262" s="3"/>
       <c r="H262" s="3"/>
@@ -12989,7 +13707,7 @@
       <c r="S262" s="1"/>
       <c r="T262" s="6"/>
     </row>
-    <row r="263" spans="6:20" ht="14.25" customHeight="1">
+    <row r="263" spans="1:20" ht="14.25" customHeight="1">
       <c r="F263" s="3"/>
       <c r="G263" s="3"/>
       <c r="H263" s="3"/>
@@ -13006,7 +13724,7 @@
       <c r="S263" s="1"/>
       <c r="T263" s="6"/>
     </row>
-    <row r="264" spans="6:20" ht="14.25" customHeight="1">
+    <row r="264" spans="1:20" ht="14.25" customHeight="1">
       <c r="F264" s="3"/>
       <c r="G264" s="3"/>
       <c r="H264" s="3"/>
@@ -13023,7 +13741,7 @@
       <c r="S264" s="1"/>
       <c r="T264" s="6"/>
     </row>
-    <row r="265" spans="6:20" ht="14.25" customHeight="1">
+    <row r="265" spans="1:20" ht="14.25" customHeight="1">
       <c r="F265" s="3"/>
       <c r="G265" s="3"/>
       <c r="H265" s="3"/>
@@ -13040,7 +13758,7 @@
       <c r="S265" s="1"/>
       <c r="T265" s="6"/>
     </row>
-    <row r="266" spans="6:20" ht="14.25" customHeight="1">
+    <row r="266" spans="1:20" ht="14.25" customHeight="1">
       <c r="F266" s="3"/>
       <c r="G266" s="3"/>
       <c r="H266" s="3"/>
@@ -13057,7 +13775,7 @@
       <c r="S266" s="1"/>
       <c r="T266" s="6"/>
     </row>
-    <row r="267" spans="6:20" ht="14.25" customHeight="1">
+    <row r="267" spans="1:20" ht="14.25" customHeight="1">
       <c r="F267" s="3"/>
       <c r="G267" s="3"/>
       <c r="H267" s="3"/>
@@ -13074,7 +13792,7 @@
       <c r="S267" s="1"/>
       <c r="T267" s="6"/>
     </row>
-    <row r="268" spans="6:20" ht="14.25" customHeight="1">
+    <row r="268" spans="1:20" ht="14.25" customHeight="1">
       <c r="F268" s="3"/>
       <c r="G268" s="3"/>
       <c r="H268" s="3"/>
@@ -13091,7 +13809,7 @@
       <c r="S268" s="1"/>
       <c r="T268" s="6"/>
     </row>
-    <row r="269" spans="6:20" ht="14.25" customHeight="1">
+    <row r="269" spans="1:20" ht="14.25" customHeight="1">
       <c r="F269" s="3"/>
       <c r="G269" s="3"/>
       <c r="H269" s="3"/>
@@ -13108,7 +13826,7 @@
       <c r="S269" s="1"/>
       <c r="T269" s="6"/>
     </row>
-    <row r="270" spans="6:20" ht="14.25" customHeight="1">
+    <row r="270" spans="1:20" ht="14.25" customHeight="1">
       <c r="F270" s="3"/>
       <c r="G270" s="3"/>
       <c r="H270" s="3"/>
@@ -13125,7 +13843,7 @@
       <c r="S270" s="1"/>
       <c r="T270" s="6"/>
     </row>
-    <row r="271" spans="6:20" ht="14.25" customHeight="1">
+    <row r="271" spans="1:20" ht="14.25" customHeight="1">
       <c r="F271" s="3"/>
       <c r="G271" s="3"/>
       <c r="H271" s="3"/>
@@ -13142,7 +13860,7 @@
       <c r="S271" s="1"/>
       <c r="T271" s="6"/>
     </row>
-    <row r="272" spans="6:20" ht="14.25" customHeight="1">
+    <row r="272" spans="1:20" ht="14.25" customHeight="1">
       <c r="F272" s="3"/>
       <c r="G272" s="3"/>
       <c r="H272" s="3"/>
@@ -22229,13 +22947,13 @@
       <c r="T859" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T241">
+  <autoFilter ref="A9:T241" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
       </filters>
     </filterColumn>
-    <sortState ref="A207:T352">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A207:T352">
       <sortCondition ref="C9:C374"/>
     </sortState>
   </autoFilter>
@@ -22249,18 +22967,18 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J191:J241 O191:O241 L191:M241 O189 L189:M189 J189 L184:M187 O184:O187 J184:J187</xm:sqref>
+          <xm:sqref>J184:J187 O191:O241 L191:M241 O189 L189:M189 J189 L184:M187 O184:O187 J191:J241</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -22273,7 +22991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>